<commit_message>
changed GPU over to the M1 chip and in process of changing code to utilize tensorflow instead of pytorch
</commit_message>
<xml_diff>
--- a/seinfeld_episode_rankings.xlsx
+++ b/seinfeld_episode_rankings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malsmith/codeup-data-science/seinfeld/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38F749F-348A-824B-8345-F76BD2C70BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1ED63-9018-B04C-BEE6-4AADE685F9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="0" windowWidth="27680" windowHeight="17440" xr2:uid="{4FF63B93-CEE8-4849-8C46-69009425F249}"/>
+    <workbookView xWindow="2020" yWindow="0" windowWidth="27680" windowHeight="17440" xr2:uid="{4FF63B93-CEE8-4849-8C46-69009425F249}"/>
   </bookViews>
   <sheets>
     <sheet name="seinfeld episode rankings" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="219">
   <si>
     <t>Title</t>
   </si>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t>the bro</t>
+  </si>
+  <si>
+    <t>assman</t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42782775-1E9A-204A-B7CE-4CC8D61671AA}">
   <dimension ref="A1:J181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4459,9 +4462,18 @@
       <c r="A105" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105">
+        <v>10</v>
+      </c>
+      <c r="D105">
+        <v>49</v>
+      </c>
       <c r="E105">
         <f>((seinfeld_episode_rankings[[#This Row],[Plot]]*seinfeld_episode_rankings[[#This Row],[Quotability/cultural impact ]])*(seinfeld_episode_rankings[[#This Row],[Laughs]]/23))</f>
-        <v>0</v>
+        <v>85.217391304347828</v>
       </c>
       <c r="F105">
         <v>8.6999999999999993</v>
@@ -4470,7 +4482,7 @@
         <v>24</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>17</v>
+        <v>218</v>
       </c>
       <c r="I105">
         <v>6</v>
@@ -4483,9 +4495,18 @@
       <c r="A106" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106">
+        <v>5</v>
+      </c>
+      <c r="D106">
+        <v>12</v>
+      </c>
       <c r="E106">
         <f>((seinfeld_episode_rankings[[#This Row],[Plot]]*seinfeld_episode_rankings[[#This Row],[Quotability/cultural impact ]])*(seinfeld_episode_rankings[[#This Row],[Laughs]]/23))</f>
-        <v>0</v>
+        <v>5.2173913043478262</v>
       </c>
       <c r="F106">
         <v>8.1</v>
@@ -4507,9 +4528,18 @@
       <c r="A107" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>9</v>
+      </c>
+      <c r="D107">
+        <v>21</v>
+      </c>
       <c r="E107">
         <f>((seinfeld_episode_rankings[[#This Row],[Plot]]*seinfeld_episode_rankings[[#This Row],[Quotability/cultural impact ]])*(seinfeld_episode_rankings[[#This Row],[Laughs]]/23))</f>
-        <v>0</v>
+        <v>24.652173913043477</v>
       </c>
       <c r="F107">
         <v>8.4</v>

</xml_diff>